<commit_message>
Publicación y S Postgrado
1- Publicación SMQ
2- Tutorización Postgrado 2023-2024
</commit_message>
<xml_diff>
--- a/data/event_en.xlsx
+++ b/data/event_en.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Grants\Datos CV\archivos (1)\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\Mile_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9D57EC-A1CB-4ABE-B4DE-0F3D429104F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EE63B4-EC74-4CE3-8F4E-149D95FBD9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>what</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Conversation eroticism on screen: between science and subjectivity</t>
+  </si>
+  <si>
+    <t>Mar. 5, 2025</t>
+  </si>
+  <si>
+    <t>International Conference on the Prevention of Sexual Abuse Perpetration: Public Health Perspectives and Challenges</t>
+  </si>
+  <si>
+    <t>\href{https://www.youtube.com/watch?v=dNqxY_fGKwE}{Universidad El Bosque}</t>
   </si>
 </sst>
 </file>
@@ -218,9 +227,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,7 +267,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -364,7 +373,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -506,7 +515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,42 +560,59 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="1" t="s">
+    <row r="5" spans="1:5" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E8" s="2"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>